<commit_message>
updates to merged_data.csv and fakedatavalidator rules
</commit_message>
<xml_diff>
--- a/code/validator/www/microplastic_images/fakedatavalidatorrules.xlsx
+++ b/code/validator/www/microplastic_images/fakedatavalidatorrules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/MooreResearchRepository/Microplastic_Data_Portal/code/validator/www/microplastic_images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87EA69B3-6527-A446-AE39-B813EA6A5598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F506DB4C-2254-7046-B4E4-0221E14297E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" xr2:uid="{15C13D03-C0F1-5840-A063-0E7DFE13566C}"/>
   </bookViews>
@@ -392,7 +392,7 @@
     <t>is.numeric(width_mm) | is.na(width_mm)</t>
   </si>
   <si>
-    <t>merged_data_sf</t>
+    <t>merged_data</t>
   </si>
 </sst>
 </file>
@@ -773,7 +773,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updates to the fakedatavalidatorrules.xlsx
</commit_message>
<xml_diff>
--- a/code/validator/www/microplastic_images/fakedatavalidatorrules.xlsx
+++ b/code/validator/www/microplastic_images/fakedatavalidatorrules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/MooreResearchRepository/Microplastic_Data_Portal/code/validator/www/microplastic_images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F506DB4C-2254-7046-B4E4-0221E14297E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB285612-D5A2-2D4C-9219-EA057973144D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" xr2:uid="{15C13D03-C0F1-5840-A063-0E7DFE13566C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{15C13D03-C0F1-5840-A063-0E7DFE13566C}"/>
   </bookViews>
   <sheets>
     <sheet name="fakedata" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="125">
   <si>
     <t>m_ps_m3</t>
   </si>
@@ -393,6 +393,24 @@
   </si>
   <si>
     <t>merged_data</t>
+  </si>
+  <si>
+    <t>latitude_new</t>
+  </si>
+  <si>
+    <t>longitude_new</t>
+  </si>
+  <si>
+    <t>The new latitude of the water system</t>
+  </si>
+  <si>
+    <t>The new longitude of the water system</t>
+  </si>
+  <si>
+    <t>grepl("^-?\\d+(\\.\\d{1,8})*$", latitude_new) &amp; !is.na(latitude_new)</t>
+  </si>
+  <si>
+    <t>grepl("^-?\\d+(\\.\\d{1,8})*$", longitude_new) &amp; !is.na(longitude_new)</t>
   </si>
 </sst>
 </file>
@@ -770,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15160A63-4DE9-0B42-81E4-0EA0E7223C57}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,13 +962,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C9" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D9">
         <v>34.460500000000003</v>
@@ -959,18 +974,15 @@
         <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C10" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D10">
         <v>-117.3646</v>
@@ -979,526 +991,566 @@
         <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C11" t="s">
         <v>118</v>
       </c>
-      <c r="D11" t="s">
-        <v>46</v>
+      <c r="D11">
+        <v>34.460500000000003</v>
       </c>
       <c r="E11" t="s">
         <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C12" t="s">
         <v>118</v>
       </c>
       <c r="D12">
-        <v>1.3348469643716601</v>
+        <v>-117.3646</v>
       </c>
       <c r="E12" t="s">
         <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="C13" t="s">
         <v>118</v>
       </c>
-      <c r="D13">
-        <v>1.5581298650002</v>
+      <c r="D13" t="s">
+        <v>46</v>
       </c>
       <c r="E13" t="s">
         <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
         <v>118</v>
       </c>
       <c r="D14">
-        <v>2.8802947927614602</v>
+        <v>1.3348469643716601</v>
       </c>
       <c r="E14" t="s">
         <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
         <v>118</v>
       </c>
       <c r="D15">
-        <v>1.64847015079911</v>
+        <v>1.5581298650002</v>
       </c>
       <c r="E15" t="s">
         <v>47</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s">
         <v>118</v>
       </c>
       <c r="D16">
-        <v>0.90015530358048201</v>
+        <v>2.8802947927614602</v>
       </c>
       <c r="E16" t="s">
         <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
         <v>118</v>
       </c>
       <c r="D17">
-        <v>2.3792953127482499</v>
+        <v>1.64847015079911</v>
       </c>
       <c r="E17" t="s">
         <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C18" t="s">
         <v>118</v>
       </c>
       <c r="D18">
-        <v>1.1956257729034501</v>
+        <v>0.90015530358048201</v>
       </c>
       <c r="E18" t="s">
         <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
         <v>118</v>
       </c>
       <c r="D19">
-        <v>4.0319763598178202</v>
+        <v>2.3792953127482499</v>
       </c>
       <c r="E19" t="s">
         <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
         <v>118</v>
       </c>
       <c r="D20">
-        <v>2.2188015999843902</v>
+        <v>1.1956257729034501</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
         <v>118</v>
       </c>
       <c r="D21">
-        <v>1.135641026524</v>
+        <v>4.0319763598178202</v>
       </c>
       <c r="E21" t="s">
         <v>47</v>
       </c>
       <c r="F21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
         <v>118</v>
       </c>
       <c r="D22">
-        <v>1.57117593287539</v>
+        <v>2.2188015999843902</v>
       </c>
       <c r="E22" t="s">
         <v>47</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
         <v>118</v>
       </c>
       <c r="D23">
-        <v>1.9547991878956399</v>
+        <v>1.135641026524</v>
       </c>
       <c r="E23" t="s">
         <v>47</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
         <v>118</v>
       </c>
       <c r="D24">
-        <v>2.76420479843501</v>
+        <v>1.57117593287539</v>
       </c>
       <c r="E24" t="s">
         <v>47</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
         <v>118</v>
       </c>
       <c r="D25">
-        <v>2.8724065826023799</v>
+        <v>1.9547991878956399</v>
       </c>
       <c r="E25" t="s">
         <v>47</v>
       </c>
       <c r="F25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
         <v>118</v>
       </c>
       <c r="D26">
-        <v>0.34125111882238701</v>
+        <v>2.76420479843501</v>
       </c>
       <c r="E26" t="s">
         <v>47</v>
       </c>
       <c r="F26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
         <v>118</v>
       </c>
       <c r="D27">
-        <v>1.5324362306118</v>
+        <v>2.8724065826023799</v>
       </c>
       <c r="E27" t="s">
         <v>47</v>
       </c>
       <c r="F27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
         <v>118</v>
       </c>
       <c r="D28">
-        <v>1.2127305941691999</v>
+        <v>0.34125111882238701</v>
       </c>
       <c r="E28" t="s">
         <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C29" t="s">
         <v>118</v>
       </c>
       <c r="D29">
-        <v>1.8473296158717301</v>
+        <v>1.5324362306118</v>
       </c>
       <c r="E29" t="s">
         <v>47</v>
       </c>
       <c r="F29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
         <v>118</v>
       </c>
       <c r="D30">
-        <v>2.5127055572114898</v>
+        <v>1.2127305941691999</v>
       </c>
       <c r="E30" t="s">
         <v>47</v>
       </c>
       <c r="F30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C31" t="s">
         <v>118</v>
       </c>
       <c r="D31">
-        <v>2.0055954093528001</v>
+        <v>1.8473296158717301</v>
       </c>
       <c r="E31" t="s">
         <v>47</v>
       </c>
       <c r="F31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C32" t="s">
         <v>118</v>
       </c>
       <c r="D32">
-        <v>0.44070426314797101</v>
+        <v>2.5127055572114898</v>
       </c>
       <c r="E32" t="s">
         <v>47</v>
       </c>
       <c r="F32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
         <v>118</v>
       </c>
       <c r="D33">
-        <v>0.844549796690654</v>
+        <v>2.0055954093528001</v>
       </c>
       <c r="E33" t="s">
         <v>47</v>
       </c>
       <c r="F33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
         <v>118</v>
       </c>
       <c r="D34">
-        <v>1.11002674679008</v>
+        <v>0.44070426314797101</v>
       </c>
       <c r="E34" t="s">
         <v>47</v>
       </c>
       <c r="F34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C35" t="s">
         <v>118</v>
       </c>
       <c r="D35">
-        <v>0.16179675020325901</v>
+        <v>0.844549796690654</v>
       </c>
       <c r="E35" t="s">
         <v>47</v>
       </c>
       <c r="F35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36">
+        <v>1.11002674679008</v>
+      </c>
+      <c r="E36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37">
+        <v>0.16179675020325901</v>
+      </c>
+      <c r="E37" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>9</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>104</v>
       </c>
-      <c r="C36" t="s">
-        <v>118</v>
-      </c>
-      <c r="D36">
+      <c r="C38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38">
         <v>1.8167456559999999</v>
       </c>
-      <c r="E36" t="s">
-        <v>47</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="E38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update to fake data validator rules (added 'merged_data' under 'dataset')
</commit_message>
<xml_diff>
--- a/code/validator/www/microplastic_images/fakedatavalidatorrules.xlsx
+++ b/code/validator/www/microplastic_images/fakedatavalidatorrules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/MooreResearchRepository/Microplastic_Data_Portal/code/validator/www/microplastic_images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB285612-D5A2-2D4C-9219-EA057973144D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{223A261D-98C3-184F-B54F-B8CB6B6DA9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{15C13D03-C0F1-5840-A063-0E7DFE13566C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="125">
   <si>
     <t>m_ps_m3</t>
   </si>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15160A63-4DE9-0B42-81E4-0EA0E7223C57}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -967,6 +967,9 @@
       <c r="B9" t="s">
         <v>121</v>
       </c>
+      <c r="C9" t="s">
+        <v>118</v>
+      </c>
       <c r="D9">
         <v>34.460500000000003</v>
       </c>
@@ -983,6 +986,9 @@
       </c>
       <c r="B10" t="s">
         <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>118</v>
       </c>
       <c r="D10">
         <v>-117.3646</v>

</xml_diff>